<commit_message>
correcting problems with names
</commit_message>
<xml_diff>
--- a/rnaSample/rnaSample_159.xlsx
+++ b/rnaSample/rnaSample_159.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/rnaSample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3C87852-4B9F-FF44-BCE1-B437F3F2D7B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A385C1FD-56DA-8A4D-9299-5333C0A3F87F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="16380" windowHeight="8200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="12">
   <si>
     <t>harvestDate</t>
   </si>
@@ -55,9 +55,6 @@
   </si>
   <si>
     <t>S.GISH</t>
-  </si>
-  <si>
-    <t>Retrofitted_159</t>
   </si>
   <si>
     <t>TRIzol</t>
@@ -496,19 +493,19 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -522,19 +519,19 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -548,19 +545,19 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4">
         <v>3</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -574,19 +571,19 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5">
         <v>4</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>